<commit_message>
added excel with variable description in R and expected sign
</commit_message>
<xml_diff>
--- a/input/full_data.xlsx
+++ b/input/full_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Viktor\Dropbox\GitHub\macroX_sovereign-yield-spreads\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8700DA1-23AF-4EB4-99CB-139E0940F209}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C901E41C-5025-40E3-A903-5CB359BF99D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="10" xr2:uid="{6BD05D62-9C8D-4B00-B784-FD56BE4060DE}"/>
   </bookViews>
@@ -22,8 +22,8 @@
     <sheet name="gcf" sheetId="5" r:id="rId7"/>
     <sheet name="tb" sheetId="13" r:id="rId8"/>
     <sheet name="tot" sheetId="8" r:id="rId9"/>
-    <sheet name="pspp" sheetId="16" r:id="rId10"/>
-    <sheet name="debt" sheetId="10" r:id="rId11"/>
+    <sheet name="debt" sheetId="10" r:id="rId10"/>
+    <sheet name="pspp" sheetId="16" r:id="rId11"/>
     <sheet name="i_us" sheetId="14" r:id="rId12"/>
     <sheet name="baa" sheetId="2" r:id="rId13"/>
     <sheet name="gdp" sheetId="4" r:id="rId14"/>
@@ -2358,14 +2358,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ABA5FCC-238B-40CE-ACE9-7FBA7AE13711}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3ACEED6-190A-4890-BB7F-1AA3A6A999CE}">
   <sheetPr>
-    <tabColor theme="7"/>
+    <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2437,61 +2437,61 @@
         <v>1999</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>279.5</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1238.5999999999999</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>0.34799999999999998</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>43.2</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>132.30000000000001</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>362.2</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>847.6</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>1331.3</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>5.43</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>0.76</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>2.89</v>
       </c>
       <c r="M2">
-        <v>0</v>
+        <v>1.66</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>2.3610000000000002</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>245.7</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>135.9</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>66.3</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>4.08</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>13.45</v>
       </c>
       <c r="T2">
-        <v>0</v>
+        <v>55.9</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -2499,61 +2499,61 @@
         <v>2000</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>281</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1245.8</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>0.316</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>39.1</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>148.19999999999999</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>374.6</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>870.6</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1353.6</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>5.91</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>0.83</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>3.14</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>1.72</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>2.5190000000000001</v>
       </c>
       <c r="O3">
-        <v>0</v>
+        <v>235.3</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <v>141.19999999999999</v>
       </c>
       <c r="Q3">
-        <v>0</v>
+        <v>69.599999999999994</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>4.8899999999999997</v>
       </c>
       <c r="S3">
-        <v>0</v>
+        <v>15.97</v>
       </c>
       <c r="T3">
-        <v>0</v>
+        <v>57.9</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -2561,61 +2561,61 @@
         <v>2001</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>286.10000000000002</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1258.7</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>40.5</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>163</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>378.9</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>897.4</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>1420</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>6.54</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>1.03</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>3.25</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>1.82</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>2.7810000000000001</v>
       </c>
       <c r="O4">
-        <v>0</v>
+        <v>238.2</v>
       </c>
       <c r="P4">
-        <v>0</v>
+        <v>147.19999999999999</v>
       </c>
       <c r="Q4">
-        <v>0</v>
+        <v>77.900000000000006</v>
       </c>
       <c r="R4">
-        <v>0</v>
+        <v>5.51</v>
       </c>
       <c r="S4">
-        <v>0</v>
+        <v>17.57</v>
       </c>
       <c r="T4">
-        <v>0</v>
+        <v>59.2</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -2623,61 +2623,61 @@
         <v>2002</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>288.10000000000002</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1312.4</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>0.443</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>41.5</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>171.4</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>384.1</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>956.8</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>1436.1</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>7.19</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>3.37</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>1.86</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>2.8519999999999999</v>
       </c>
       <c r="O5">
-        <v>0</v>
+        <v>244.5</v>
       </c>
       <c r="P5">
-        <v>0</v>
+        <v>151.30000000000001</v>
       </c>
       <c r="Q5">
-        <v>0</v>
+        <v>85.6</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <v>6.44</v>
       </c>
       <c r="S5">
-        <v>0</v>
+        <v>16.91</v>
       </c>
       <c r="T5">
-        <v>0</v>
+        <v>59.7</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -2685,61 +2685,61 @@
         <v>2003</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>285.89999999999998</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1400.1</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>0.49</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>43.6</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>181.5</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>382.8</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>1050.4000000000001</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>1471.3</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>3.39</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>1.95</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>3.286</v>
       </c>
       <c r="O6">
-        <v>0</v>
+        <v>256.3</v>
       </c>
       <c r="P6">
-        <v>0</v>
+        <v>152.69999999999999</v>
       </c>
       <c r="Q6">
-        <v>0</v>
+        <v>93.3</v>
       </c>
       <c r="R6">
-        <v>0</v>
+        <v>6.86</v>
       </c>
       <c r="S6">
-        <v>0</v>
+        <v>17.940000000000001</v>
       </c>
       <c r="T6">
-        <v>0</v>
+        <v>64.900000000000006</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -2747,61 +2747,61 @@
         <v>2004</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>288.39999999999998</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1470.4</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>44.1</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>199.3</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>389.9</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>1123.5999999999999</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>1526.4</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>8.9700000000000006</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>1.62</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>3.4</v>
       </c>
       <c r="M7">
-        <v>0</v>
+        <v>2.21</v>
       </c>
       <c r="N7">
-        <v>0</v>
+        <v>3.49</v>
       </c>
       <c r="O7">
-        <v>0</v>
+        <v>266.10000000000002</v>
       </c>
       <c r="P7">
-        <v>0</v>
+        <v>158</v>
       </c>
       <c r="Q7">
-        <v>0</v>
+        <v>102.2</v>
       </c>
       <c r="R7">
-        <v>0</v>
+        <v>7.43</v>
       </c>
       <c r="S7">
-        <v>0</v>
+        <v>19.260000000000002</v>
       </c>
       <c r="T7">
-        <v>0</v>
+        <v>67.7</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -2809,61 +2809,61 @@
         <v>2005</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>295</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1541.1</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>0.53300000000000003</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>44.4</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>214</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>393.5</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>1189.9000000000001</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>1591.6</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>9.4</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>1.62</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>3.7</v>
       </c>
       <c r="M8">
-        <v>0</v>
+        <v>2.41</v>
       </c>
       <c r="N8">
-        <v>0</v>
+        <v>3.6059999999999999</v>
       </c>
       <c r="O8">
-        <v>0</v>
+        <v>274.3</v>
       </c>
       <c r="P8">
-        <v>0</v>
+        <v>174.4</v>
       </c>
       <c r="Q8">
-        <v>0</v>
+        <v>114.6</v>
       </c>
       <c r="R8">
-        <v>0</v>
+        <v>7.69</v>
       </c>
       <c r="S8">
-        <v>0</v>
+        <v>17.53</v>
       </c>
       <c r="T8">
-        <v>0</v>
+        <v>65.8</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -2871,61 +2871,61 @@
         <v>2006</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>297.5</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1591</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>0.628</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>43.7</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>225.7</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>392.1</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>1194.0999999999999</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>1657.4</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>9.48</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>1.72</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="M9">
-        <v>0</v>
+        <v>2.81</v>
       </c>
       <c r="N9">
-        <v>0</v>
+        <v>3.4729999999999999</v>
       </c>
       <c r="O9">
-        <v>0</v>
+        <v>264.2</v>
       </c>
       <c r="P9">
-        <v>0</v>
+        <v>180.3</v>
       </c>
       <c r="Q9">
-        <v>0</v>
+        <v>122.5</v>
       </c>
       <c r="R9">
-        <v>0</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="S9">
-        <v>0</v>
+        <v>17.71</v>
       </c>
       <c r="T9">
-        <v>0</v>
+        <v>65.900000000000006</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -2933,61 +2933,61 @@
         <v>2007</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>300.10000000000002</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1599.6</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>0.61799999999999999</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>47.1</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>239.9</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>384.7</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>1252.9000000000001</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>1677.7</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>9.4600000000000009</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <v>1.92</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>4.6100000000000003</v>
       </c>
       <c r="M10">
-        <v>0</v>
+        <v>3.05</v>
       </c>
       <c r="N10">
-        <v>0</v>
+        <v>3.585</v>
       </c>
       <c r="O10">
-        <v>0</v>
+        <v>266.10000000000002</v>
       </c>
       <c r="P10">
-        <v>0</v>
+        <v>184.7</v>
       </c>
       <c r="Q10">
-        <v>0</v>
+        <v>127.6</v>
       </c>
       <c r="R10">
-        <v>0</v>
+        <v>8.01</v>
       </c>
       <c r="S10">
-        <v>0</v>
+        <v>19.170000000000002</v>
       </c>
       <c r="T10">
-        <v>0</v>
+        <v>63.4</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -2995,61 +2995,61 @@
         <v>2008</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>327.7</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1668.5</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>0.749</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>79.599999999999994</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>264.8</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>440.6</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>1370.3</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>1738.5</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>8.66</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>4.55</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>4.76</v>
       </c>
       <c r="M11">
-        <v>0</v>
+        <v>5.86</v>
       </c>
       <c r="N11">
-        <v>0</v>
+        <v>3.8370000000000002</v>
       </c>
       <c r="O11">
-        <v>0</v>
+        <v>353.9</v>
       </c>
       <c r="P11">
-        <v>0</v>
+        <v>201.8</v>
       </c>
       <c r="Q11">
-        <v>0</v>
+        <v>135.5</v>
       </c>
       <c r="R11">
-        <v>0</v>
+        <v>8.26</v>
       </c>
       <c r="S11">
-        <v>0</v>
+        <v>19.62</v>
       </c>
       <c r="T11">
-        <v>0</v>
+        <v>63.3</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -3057,61 +3057,61 @@
         <v>2009</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>347.2</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>1785.1</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>1.0229999999999999</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>104.7</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>301.10000000000002</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>569.5</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>1608</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>1839.1</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>10.14</v>
       </c>
       <c r="K12">
-        <v>0</v>
+        <v>6.98</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>7.53</v>
       </c>
       <c r="M12">
-        <v>0</v>
+        <v>5.97</v>
       </c>
       <c r="N12">
-        <v>0</v>
+        <v>4.1529999999999996</v>
       </c>
       <c r="O12">
-        <v>0</v>
+        <v>354.7</v>
       </c>
       <c r="P12">
-        <v>0</v>
+        <v>230</v>
       </c>
       <c r="Q12">
-        <v>0</v>
+        <v>154</v>
       </c>
       <c r="R12">
-        <v>0</v>
+        <v>12.52</v>
       </c>
       <c r="S12">
-        <v>0</v>
+        <v>23.31</v>
       </c>
       <c r="T12">
-        <v>0</v>
+        <v>75.5</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -3119,61 +3119,61 @@
         <v>2010</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>364.1</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>2112.6</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>0.98199999999999998</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>144.19999999999999</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>330.6</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>649.20000000000005</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>1701.1</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>1920.7</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>10.95</v>
       </c>
       <c r="K13">
-        <v>0</v>
+        <v>8.64</v>
       </c>
       <c r="L13">
-        <v>0</v>
+        <v>10.15</v>
       </c>
       <c r="M13">
-        <v>0</v>
+        <v>8.1</v>
       </c>
       <c r="N13">
-        <v>0</v>
+        <v>4.452</v>
       </c>
       <c r="O13">
-        <v>0</v>
+        <v>378.7</v>
       </c>
       <c r="P13">
-        <v>0</v>
+        <v>244.7</v>
       </c>
       <c r="Q13">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="R13">
-        <v>0</v>
+        <v>13.92</v>
       </c>
       <c r="S13">
-        <v>0</v>
+        <v>27.91</v>
       </c>
       <c r="T13">
-        <v>0</v>
+        <v>88.2</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
@@ -3181,61 +3181,61 @@
         <v>2011</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>389.1</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>2149.5</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>1.0269999999999999</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>189.7</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>356.2</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>743</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>1808</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>1973.5</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>13.06</v>
       </c>
       <c r="K14">
-        <v>0</v>
+        <v>8.91</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>11.63</v>
       </c>
       <c r="M14">
-        <v>0</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="N14">
-        <v>0</v>
+        <v>4.7969999999999997</v>
       </c>
       <c r="O14">
-        <v>0</v>
+        <v>401.2</v>
       </c>
       <c r="P14">
-        <v>0</v>
+        <v>255.7</v>
       </c>
       <c r="Q14">
-        <v>0</v>
+        <v>201.5</v>
       </c>
       <c r="R14">
-        <v>0</v>
+        <v>17.22</v>
       </c>
       <c r="S14">
-        <v>0</v>
+        <v>30.95</v>
       </c>
       <c r="T14">
-        <v>0</v>
+        <v>95.6</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
@@ -3243,61 +3243,61 @@
         <v>2012</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>404.8</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>2227.4</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1.7629999999999999</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>210</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>305.10000000000002</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>889.9</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>1892.5</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>2054.8000000000002</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>15.62</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="L15">
-        <v>0</v>
+        <v>13.26</v>
       </c>
       <c r="M15">
-        <v>0</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="N15">
-        <v>0</v>
+        <v>4.8550000000000004</v>
       </c>
       <c r="O15">
-        <v>0</v>
+        <v>432.4</v>
       </c>
       <c r="P15">
-        <v>0</v>
+        <v>261</v>
       </c>
       <c r="Q15">
-        <v>0</v>
+        <v>217.2</v>
       </c>
       <c r="R15">
-        <v>0</v>
+        <v>19.420000000000002</v>
       </c>
       <c r="S15">
-        <v>0</v>
+        <v>38.03</v>
       </c>
       <c r="T15">
-        <v>0</v>
+        <v>107.8</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -3305,61 +3305,61 @@
         <v>2013</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>414.4</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>2213</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>1.9339999999999999</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>215.4</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>320.5</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>977.3</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>1977.7</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>2136.1999999999998</v>
       </c>
       <c r="J16">
-        <v>0</v>
+        <v>18.71</v>
       </c>
       <c r="K16">
-        <v>0</v>
+        <v>9.18</v>
       </c>
       <c r="L16">
-        <v>0</v>
+        <v>13.55</v>
       </c>
       <c r="M16">
-        <v>0</v>
+        <v>11.01</v>
       </c>
       <c r="N16">
-        <v>0</v>
+        <v>5.2270000000000003</v>
       </c>
       <c r="O16">
-        <v>0</v>
+        <v>446.8</v>
       </c>
       <c r="P16">
-        <v>0</v>
+        <v>263.2</v>
       </c>
       <c r="Q16">
-        <v>0</v>
+        <v>224.1</v>
       </c>
       <c r="R16">
-        <v>0</v>
+        <v>25.52</v>
       </c>
       <c r="S16">
-        <v>0</v>
+        <v>40.68</v>
       </c>
       <c r="T16">
-        <v>0</v>
+        <v>114.9</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
@@ -3367,371 +3367,371 @@
         <v>2014</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>431.2</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>2215.1999999999998</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>2.13</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>203.4</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>319.60000000000002</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>1039.4000000000001</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>2039.9</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <v>2203</v>
       </c>
       <c r="J17">
-        <v>0</v>
+        <v>19.010000000000002</v>
       </c>
       <c r="K17">
-        <v>0</v>
+        <v>9.83</v>
       </c>
       <c r="L17">
-        <v>0</v>
+        <v>14.83</v>
       </c>
       <c r="M17">
-        <v>0</v>
+        <v>11.33</v>
       </c>
       <c r="N17">
-        <v>0</v>
+        <v>5.39</v>
       </c>
       <c r="O17">
-        <v>0</v>
+        <v>455.6</v>
       </c>
       <c r="P17">
-        <v>0</v>
+        <v>280</v>
       </c>
       <c r="Q17">
-        <v>0</v>
+        <v>230.1</v>
       </c>
       <c r="R17">
-        <v>0</v>
+        <v>30.22</v>
       </c>
       <c r="S17">
-        <v>0</v>
+        <v>40.799999999999997</v>
       </c>
       <c r="T17">
-        <v>0</v>
+        <v>123.8</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2015</v>
       </c>
-      <c r="B18" s="2">
-        <v>12641</v>
-      </c>
-      <c r="C18" s="2">
-        <v>115625</v>
-      </c>
-      <c r="D18" s="2">
-        <v>48</v>
-      </c>
-      <c r="E18" s="2">
-        <v>7583</v>
-      </c>
-      <c r="F18" s="2">
-        <v>0</v>
-      </c>
-      <c r="G18" s="2">
-        <v>56817</v>
-      </c>
-      <c r="H18" s="2">
-        <v>91767</v>
-      </c>
-      <c r="I18" s="2">
-        <v>79209</v>
-      </c>
-      <c r="J18" s="2">
-        <v>285</v>
-      </c>
-      <c r="K18" s="2">
-        <v>684</v>
-      </c>
-      <c r="L18" s="2">
-        <v>1107</v>
-      </c>
-      <c r="M18" s="2">
-        <v>1115</v>
-      </c>
-      <c r="N18" s="2">
-        <v>282</v>
-      </c>
-      <c r="O18" s="2">
-        <v>25612</v>
-      </c>
-      <c r="P18" s="2">
-        <v>12641</v>
-      </c>
-      <c r="Q18" s="2">
-        <v>11220</v>
-      </c>
-      <c r="R18" s="2">
-        <v>2228</v>
-      </c>
-      <c r="S18" s="2">
-        <v>4622</v>
-      </c>
-      <c r="T18" s="2">
-        <v>8086</v>
+      <c r="B18">
+        <v>438.2</v>
+      </c>
+      <c r="C18">
+        <v>2185.1</v>
+      </c>
+      <c r="D18">
+        <v>2.077</v>
+      </c>
+      <c r="E18">
+        <v>201.6</v>
+      </c>
+      <c r="F18">
+        <v>311.7</v>
+      </c>
+      <c r="G18">
+        <v>1070.0999999999999</v>
+      </c>
+      <c r="H18">
+        <v>2101.3000000000002</v>
+      </c>
+      <c r="I18">
+        <v>2239.4</v>
+      </c>
+      <c r="J18">
+        <v>19.16</v>
+      </c>
+      <c r="K18">
+        <v>9.11</v>
+      </c>
+      <c r="L18">
+        <v>15.88</v>
+      </c>
+      <c r="M18">
+        <v>11.45</v>
+      </c>
+      <c r="N18">
+        <v>5.5860000000000003</v>
+      </c>
+      <c r="O18">
+        <v>446</v>
+      </c>
+      <c r="P18">
+        <v>292.3</v>
+      </c>
+      <c r="Q18">
+        <v>235.7</v>
+      </c>
+      <c r="R18">
+        <v>32.090000000000003</v>
+      </c>
+      <c r="S18">
+        <v>41.38</v>
+      </c>
+      <c r="T18">
+        <v>134.5</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2016</v>
       </c>
-      <c r="B19" s="2">
-        <v>20559</v>
-      </c>
-      <c r="C19" s="2">
-        <v>188321</v>
-      </c>
-      <c r="D19" s="2">
-        <v>18</v>
-      </c>
-      <c r="E19" s="2">
-        <v>10982</v>
-      </c>
-      <c r="F19" s="2">
-        <v>0</v>
-      </c>
-      <c r="G19" s="2">
-        <v>93514</v>
-      </c>
-      <c r="H19" s="2">
-        <v>149100</v>
-      </c>
-      <c r="I19" s="2">
-        <v>130398</v>
-      </c>
-      <c r="J19" s="2">
-        <v>-37</v>
-      </c>
-      <c r="K19" s="2">
-        <v>628</v>
-      </c>
-      <c r="L19" s="2">
-        <v>1157</v>
-      </c>
-      <c r="M19" s="2">
-        <v>628</v>
-      </c>
-      <c r="N19" s="2">
-        <v>525</v>
-      </c>
-      <c r="O19" s="2">
-        <v>42212</v>
-      </c>
-      <c r="P19" s="2">
-        <v>20559</v>
-      </c>
-      <c r="Q19" s="2">
-        <v>13390</v>
-      </c>
-      <c r="R19" s="2">
-        <v>2705</v>
-      </c>
-      <c r="S19" s="2">
-        <v>3534</v>
-      </c>
-      <c r="T19" s="2">
-        <v>13205</v>
+      <c r="B19">
+        <v>451.3</v>
+      </c>
+      <c r="C19">
+        <v>2169</v>
+      </c>
+      <c r="D19">
+        <v>2.2160000000000002</v>
+      </c>
+      <c r="E19">
+        <v>200.6</v>
+      </c>
+      <c r="F19">
+        <v>315</v>
+      </c>
+      <c r="G19">
+        <v>1104.5999999999999</v>
+      </c>
+      <c r="H19">
+        <v>2188.5</v>
+      </c>
+      <c r="I19">
+        <v>2285.6</v>
+      </c>
+      <c r="J19">
+        <v>19.510000000000002</v>
+      </c>
+      <c r="K19">
+        <v>10.25</v>
+      </c>
+      <c r="L19">
+        <v>15.45</v>
+      </c>
+      <c r="M19">
+        <v>11.02</v>
+      </c>
+      <c r="N19">
+        <v>5.74</v>
+      </c>
+      <c r="O19">
+        <v>438.4</v>
+      </c>
+      <c r="P19">
+        <v>296.3</v>
+      </c>
+      <c r="Q19">
+        <v>245.2</v>
+      </c>
+      <c r="R19">
+        <v>31.76</v>
+      </c>
+      <c r="S19">
+        <v>42.16</v>
+      </c>
+      <c r="T19">
+        <v>137.4</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2017</v>
       </c>
-      <c r="B20" s="2">
-        <v>18761</v>
-      </c>
-      <c r="C20" s="2">
-        <v>155372</v>
-      </c>
-      <c r="D20" s="2">
-        <v>0</v>
-      </c>
-      <c r="E20" s="2">
-        <v>6719</v>
-      </c>
-      <c r="F20" s="2">
-        <v>0</v>
-      </c>
-      <c r="G20" s="2">
-        <v>79919</v>
-      </c>
-      <c r="H20" s="2">
-        <v>134836</v>
-      </c>
-      <c r="I20" s="2">
-        <v>117120</v>
-      </c>
-      <c r="J20" s="2">
-        <v>-35</v>
-      </c>
-      <c r="K20" s="2">
-        <v>430</v>
-      </c>
-      <c r="L20" s="2">
-        <v>640</v>
-      </c>
-      <c r="M20" s="2">
-        <v>642</v>
-      </c>
-      <c r="N20" s="2">
-        <v>220</v>
-      </c>
-      <c r="O20" s="2">
-        <v>34959</v>
-      </c>
-      <c r="P20" s="2">
-        <v>18761</v>
-      </c>
-      <c r="Q20" s="2">
-        <v>6464</v>
-      </c>
-      <c r="R20" s="2">
-        <v>1974</v>
-      </c>
-      <c r="S20" s="2">
-        <v>2627</v>
-      </c>
-      <c r="T20" s="2">
-        <v>7872</v>
+      <c r="B20">
+        <v>453.8</v>
+      </c>
+      <c r="C20">
+        <v>2118.6999999999998</v>
+      </c>
+      <c r="D20">
+        <v>2.2189999999999999</v>
+      </c>
+      <c r="E20">
+        <v>201.3</v>
+      </c>
+      <c r="F20">
+        <v>317.5</v>
+      </c>
+      <c r="G20">
+        <v>1145.0999999999999</v>
+      </c>
+      <c r="H20">
+        <v>2258.6</v>
+      </c>
+      <c r="I20">
+        <v>2329.6</v>
+      </c>
+      <c r="J20">
+        <v>18.809999999999999</v>
+      </c>
+      <c r="K20">
+        <v>10.52</v>
+      </c>
+      <c r="L20">
+        <v>16.54</v>
+      </c>
+      <c r="M20">
+        <v>12.7</v>
+      </c>
+      <c r="N20">
+        <v>5.6779999999999999</v>
+      </c>
+      <c r="O20">
+        <v>420.1</v>
+      </c>
+      <c r="P20">
+        <v>289.89999999999998</v>
+      </c>
+      <c r="Q20">
+        <v>247.2</v>
+      </c>
+      <c r="R20">
+        <v>31.86</v>
+      </c>
+      <c r="S20">
+        <v>43.37</v>
+      </c>
+      <c r="T20">
+        <v>138.4</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2018</v>
       </c>
-      <c r="B21" s="2">
-        <v>6228</v>
-      </c>
-      <c r="C21" s="2">
-        <v>59239</v>
-      </c>
-      <c r="D21" s="2">
-        <v>-58</v>
-      </c>
-      <c r="E21" s="2">
-        <v>4851</v>
-      </c>
-      <c r="F21" s="2">
-        <v>0</v>
-      </c>
-      <c r="G21" s="2">
-        <v>30571</v>
-      </c>
-      <c r="H21" s="2">
-        <v>44554</v>
-      </c>
-      <c r="I21" s="2">
-        <v>38627</v>
-      </c>
-      <c r="J21" s="2">
-        <v>464</v>
-      </c>
-      <c r="K21" s="2">
-        <v>333</v>
-      </c>
-      <c r="L21" s="2">
-        <v>260</v>
-      </c>
-      <c r="M21" s="2">
-        <v>228</v>
-      </c>
-      <c r="N21" s="2">
-        <v>127</v>
-      </c>
-      <c r="O21" s="2">
-        <v>12400</v>
-      </c>
-      <c r="P21" s="2">
-        <v>6228</v>
-      </c>
-      <c r="Q21" s="2">
-        <v>5772</v>
-      </c>
-      <c r="R21" s="2">
-        <v>1039</v>
-      </c>
-      <c r="S21" s="2">
-        <v>902</v>
-      </c>
-      <c r="T21" s="2">
-        <v>3970</v>
+      <c r="B21">
+        <v>459.1</v>
+      </c>
+      <c r="C21">
+        <v>2068.6</v>
+      </c>
+      <c r="D21">
+        <v>2.1739999999999999</v>
+      </c>
+      <c r="E21">
+        <v>205.9</v>
+      </c>
+      <c r="F21">
+        <v>334.7</v>
+      </c>
+      <c r="G21">
+        <v>1173.3</v>
+      </c>
+      <c r="H21">
+        <v>2314.9</v>
+      </c>
+      <c r="I21">
+        <v>2380.9</v>
+      </c>
+      <c r="J21">
+        <v>21.26</v>
+      </c>
+      <c r="K21">
+        <v>10.82</v>
+      </c>
+      <c r="L21">
+        <v>15.32</v>
+      </c>
+      <c r="M21">
+        <v>12.61</v>
+      </c>
+      <c r="N21">
+        <v>5.6440000000000001</v>
+      </c>
+      <c r="O21">
+        <v>405.5</v>
+      </c>
+      <c r="P21">
+        <v>285.3</v>
+      </c>
+      <c r="Q21">
+        <v>249.3</v>
+      </c>
+      <c r="R21">
+        <v>32.22</v>
+      </c>
+      <c r="S21">
+        <v>44.32</v>
+      </c>
+      <c r="T21">
+        <v>139.30000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2019</v>
       </c>
-      <c r="B22" s="2">
-        <v>1387</v>
-      </c>
-      <c r="C22" s="2">
-        <v>9276</v>
-      </c>
-      <c r="D22" s="2">
-        <v>0</v>
-      </c>
-      <c r="E22" s="2">
-        <v>2591</v>
-      </c>
-      <c r="F22" s="2">
-        <v>0</v>
-      </c>
-      <c r="G22" s="2">
-        <v>-1819</v>
-      </c>
-      <c r="H22" s="2">
-        <v>4904</v>
-      </c>
-      <c r="I22" s="2">
-        <v>-1566</v>
-      </c>
-      <c r="J22" s="2">
-        <v>1267</v>
-      </c>
-      <c r="K22" s="2">
-        <v>282</v>
-      </c>
-      <c r="L22" s="2">
-        <v>541</v>
-      </c>
-      <c r="M22" s="2">
-        <v>107</v>
-      </c>
-      <c r="N22" s="2">
-        <v>-1</v>
-      </c>
-      <c r="O22" s="2">
-        <v>-421</v>
-      </c>
-      <c r="P22" s="2">
-        <v>1387</v>
-      </c>
-      <c r="Q22" s="2">
-        <v>4343</v>
-      </c>
-      <c r="R22" s="2">
-        <v>263</v>
-      </c>
-      <c r="S22" s="2">
-        <v>837</v>
-      </c>
-      <c r="T22" s="2">
-        <v>751</v>
+      <c r="B22">
+        <v>467.2</v>
+      </c>
+      <c r="C22">
+        <v>2053</v>
+      </c>
+      <c r="D22">
+        <v>2.36</v>
+      </c>
+      <c r="E22">
+        <v>204</v>
+      </c>
+      <c r="F22">
+        <v>331.1</v>
+      </c>
+      <c r="G22">
+        <v>1188.9000000000001</v>
+      </c>
+      <c r="H22">
+        <v>2380.1</v>
+      </c>
+      <c r="I22">
+        <v>2409.8000000000002</v>
+      </c>
+      <c r="J22">
+        <v>20.96</v>
+      </c>
+      <c r="K22">
+        <v>11.24</v>
+      </c>
+      <c r="L22">
+        <v>17.52</v>
+      </c>
+      <c r="M22">
+        <v>14.01</v>
+      </c>
+      <c r="N22">
+        <v>5.6959999999999997</v>
+      </c>
+      <c r="O22">
+        <v>394.6</v>
+      </c>
+      <c r="P22">
+        <v>280.39999999999998</v>
+      </c>
+      <c r="Q22">
+        <v>250</v>
+      </c>
+      <c r="R22">
+        <v>31.74</v>
+      </c>
+      <c r="S22">
+        <v>45.2</v>
+      </c>
+      <c r="T22">
+        <v>142.5</v>
       </c>
     </row>
   </sheetData>
@@ -3740,14 +3740,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3ACEED6-190A-4890-BB7F-1AA3A6A999CE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ABA5FCC-238B-40CE-ACE9-7FBA7AE13711}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3819,61 +3819,61 @@
         <v>1999</v>
       </c>
       <c r="B2">
-        <v>279.5</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>1238.5999999999999</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>0.34799999999999998</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>43.2</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>132.30000000000001</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>362.2</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>847.6</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>1331.3</v>
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>5.43</v>
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>0.76</v>
+        <v>0</v>
       </c>
       <c r="L2">
-        <v>2.89</v>
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>1.66</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>2.3610000000000002</v>
+        <v>0</v>
       </c>
       <c r="O2">
-        <v>245.7</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>135.9</v>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <v>66.3</v>
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>4.08</v>
+        <v>0</v>
       </c>
       <c r="S2">
-        <v>13.45</v>
+        <v>0</v>
       </c>
       <c r="T2">
-        <v>55.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -3881,61 +3881,61 @@
         <v>2000</v>
       </c>
       <c r="B3">
-        <v>281</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>1245.8</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>0.316</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>39.1</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>148.19999999999999</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>374.6</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>870.6</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>1353.6</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <v>5.91</v>
+        <v>0</v>
       </c>
       <c r="K3">
-        <v>0.83</v>
+        <v>0</v>
       </c>
       <c r="L3">
-        <v>3.14</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>1.72</v>
+        <v>0</v>
       </c>
       <c r="N3">
-        <v>2.5190000000000001</v>
+        <v>0</v>
       </c>
       <c r="O3">
-        <v>235.3</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>141.19999999999999</v>
+        <v>0</v>
       </c>
       <c r="Q3">
-        <v>69.599999999999994</v>
+        <v>0</v>
       </c>
       <c r="R3">
-        <v>4.8899999999999997</v>
+        <v>0</v>
       </c>
       <c r="S3">
-        <v>15.97</v>
+        <v>0</v>
       </c>
       <c r="T3">
-        <v>57.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -3943,61 +3943,61 @@
         <v>2001</v>
       </c>
       <c r="B4">
-        <v>286.10000000000002</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>1258.7</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>0.33300000000000002</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>40.5</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>163</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>378.9</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>897.4</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>1420</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <v>6.54</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>1.03</v>
+        <v>0</v>
       </c>
       <c r="L4">
-        <v>3.25</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>1.82</v>
+        <v>0</v>
       </c>
       <c r="N4">
-        <v>2.7810000000000001</v>
+        <v>0</v>
       </c>
       <c r="O4">
-        <v>238.2</v>
+        <v>0</v>
       </c>
       <c r="P4">
-        <v>147.19999999999999</v>
+        <v>0</v>
       </c>
       <c r="Q4">
-        <v>77.900000000000006</v>
+        <v>0</v>
       </c>
       <c r="R4">
-        <v>5.51</v>
+        <v>0</v>
       </c>
       <c r="S4">
-        <v>17.57</v>
+        <v>0</v>
       </c>
       <c r="T4">
-        <v>59.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -4005,61 +4005,61 @@
         <v>2002</v>
       </c>
       <c r="B5">
-        <v>288.10000000000002</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>1312.4</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>0.443</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>41.5</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>171.4</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>384.1</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>956.8</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>1436.1</v>
+        <v>0</v>
       </c>
       <c r="J5">
-        <v>7.19</v>
+        <v>0</v>
       </c>
       <c r="K5">
-        <v>1.0900000000000001</v>
+        <v>0</v>
       </c>
       <c r="L5">
-        <v>3.37</v>
+        <v>0</v>
       </c>
       <c r="M5">
-        <v>1.86</v>
+        <v>0</v>
       </c>
       <c r="N5">
-        <v>2.8519999999999999</v>
+        <v>0</v>
       </c>
       <c r="O5">
-        <v>244.5</v>
+        <v>0</v>
       </c>
       <c r="P5">
-        <v>151.30000000000001</v>
+        <v>0</v>
       </c>
       <c r="Q5">
-        <v>85.6</v>
+        <v>0</v>
       </c>
       <c r="R5">
-        <v>6.44</v>
+        <v>0</v>
       </c>
       <c r="S5">
-        <v>16.91</v>
+        <v>0</v>
       </c>
       <c r="T5">
-        <v>59.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -4067,61 +4067,61 @@
         <v>2003</v>
       </c>
       <c r="B6">
-        <v>285.89999999999998</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>1400.1</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>0.49</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>43.6</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>181.5</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>382.8</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>1050.4000000000001</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <v>1471.3</v>
+        <v>0</v>
       </c>
       <c r="J6">
-        <v>8.1999999999999993</v>
+        <v>0</v>
       </c>
       <c r="K6">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="L6">
-        <v>3.39</v>
+        <v>0</v>
       </c>
       <c r="M6">
-        <v>1.95</v>
+        <v>0</v>
       </c>
       <c r="N6">
-        <v>3.286</v>
+        <v>0</v>
       </c>
       <c r="O6">
-        <v>256.3</v>
+        <v>0</v>
       </c>
       <c r="P6">
-        <v>152.69999999999999</v>
+        <v>0</v>
       </c>
       <c r="Q6">
-        <v>93.3</v>
+        <v>0</v>
       </c>
       <c r="R6">
-        <v>6.86</v>
+        <v>0</v>
       </c>
       <c r="S6">
-        <v>17.940000000000001</v>
+        <v>0</v>
       </c>
       <c r="T6">
-        <v>64.900000000000006</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -4129,61 +4129,61 @@
         <v>2004</v>
       </c>
       <c r="B7">
-        <v>288.39999999999998</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>1470.4</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>44.1</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>199.3</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>389.9</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <v>1123.5999999999999</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>1526.4</v>
+        <v>0</v>
       </c>
       <c r="J7">
-        <v>8.9700000000000006</v>
+        <v>0</v>
       </c>
       <c r="K7">
-        <v>1.62</v>
+        <v>0</v>
       </c>
       <c r="L7">
-        <v>3.4</v>
+        <v>0</v>
       </c>
       <c r="M7">
-        <v>2.21</v>
+        <v>0</v>
       </c>
       <c r="N7">
-        <v>3.49</v>
+        <v>0</v>
       </c>
       <c r="O7">
-        <v>266.10000000000002</v>
+        <v>0</v>
       </c>
       <c r="P7">
-        <v>158</v>
+        <v>0</v>
       </c>
       <c r="Q7">
-        <v>102.2</v>
+        <v>0</v>
       </c>
       <c r="R7">
-        <v>7.43</v>
+        <v>0</v>
       </c>
       <c r="S7">
-        <v>19.260000000000002</v>
+        <v>0</v>
       </c>
       <c r="T7">
-        <v>67.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -4191,61 +4191,61 @@
         <v>2005</v>
       </c>
       <c r="B8">
-        <v>295</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>1541.1</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>0.53300000000000003</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>44.4</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>214</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>393.5</v>
+        <v>0</v>
       </c>
       <c r="H8">
-        <v>1189.9000000000001</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>1591.6</v>
+        <v>0</v>
       </c>
       <c r="J8">
-        <v>9.4</v>
+        <v>0</v>
       </c>
       <c r="K8">
-        <v>1.62</v>
+        <v>0</v>
       </c>
       <c r="L8">
-        <v>3.7</v>
+        <v>0</v>
       </c>
       <c r="M8">
-        <v>2.41</v>
+        <v>0</v>
       </c>
       <c r="N8">
-        <v>3.6059999999999999</v>
+        <v>0</v>
       </c>
       <c r="O8">
-        <v>274.3</v>
+        <v>0</v>
       </c>
       <c r="P8">
-        <v>174.4</v>
+        <v>0</v>
       </c>
       <c r="Q8">
-        <v>114.6</v>
+        <v>0</v>
       </c>
       <c r="R8">
-        <v>7.69</v>
+        <v>0</v>
       </c>
       <c r="S8">
-        <v>17.53</v>
+        <v>0</v>
       </c>
       <c r="T8">
-        <v>65.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -4253,61 +4253,61 @@
         <v>2006</v>
       </c>
       <c r="B9">
-        <v>297.5</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>1591</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>0.628</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>43.7</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>225.7</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>392.1</v>
+        <v>0</v>
       </c>
       <c r="H9">
-        <v>1194.0999999999999</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <v>1657.4</v>
+        <v>0</v>
       </c>
       <c r="J9">
-        <v>9.48</v>
+        <v>0</v>
       </c>
       <c r="K9">
-        <v>1.72</v>
+        <v>0</v>
       </c>
       <c r="L9">
-        <v>4.1500000000000004</v>
+        <v>0</v>
       </c>
       <c r="M9">
-        <v>2.81</v>
+        <v>0</v>
       </c>
       <c r="N9">
-        <v>3.4729999999999999</v>
+        <v>0</v>
       </c>
       <c r="O9">
-        <v>264.2</v>
+        <v>0</v>
       </c>
       <c r="P9">
-        <v>180.3</v>
+        <v>0</v>
       </c>
       <c r="Q9">
-        <v>122.5</v>
+        <v>0</v>
       </c>
       <c r="R9">
-        <v>8.1999999999999993</v>
+        <v>0</v>
       </c>
       <c r="S9">
-        <v>17.71</v>
+        <v>0</v>
       </c>
       <c r="T9">
-        <v>65.900000000000006</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -4315,61 +4315,61 @@
         <v>2007</v>
       </c>
       <c r="B10">
-        <v>300.10000000000002</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>1599.6</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>0.61799999999999999</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>47.1</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>239.9</v>
+        <v>0</v>
       </c>
       <c r="G10">
-        <v>384.7</v>
+        <v>0</v>
       </c>
       <c r="H10">
-        <v>1252.9000000000001</v>
+        <v>0</v>
       </c>
       <c r="I10">
-        <v>1677.7</v>
+        <v>0</v>
       </c>
       <c r="J10">
-        <v>9.4600000000000009</v>
+        <v>0</v>
       </c>
       <c r="K10">
-        <v>1.92</v>
+        <v>0</v>
       </c>
       <c r="L10">
-        <v>4.6100000000000003</v>
+        <v>0</v>
       </c>
       <c r="M10">
-        <v>3.05</v>
+        <v>0</v>
       </c>
       <c r="N10">
-        <v>3.585</v>
+        <v>0</v>
       </c>
       <c r="O10">
-        <v>266.10000000000002</v>
+        <v>0</v>
       </c>
       <c r="P10">
-        <v>184.7</v>
+        <v>0</v>
       </c>
       <c r="Q10">
-        <v>127.6</v>
+        <v>0</v>
       </c>
       <c r="R10">
-        <v>8.01</v>
+        <v>0</v>
       </c>
       <c r="S10">
-        <v>19.170000000000002</v>
+        <v>0</v>
       </c>
       <c r="T10">
-        <v>63.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -4377,61 +4377,61 @@
         <v>2008</v>
       </c>
       <c r="B11">
-        <v>327.7</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>1668.5</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>0.749</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>79.599999999999994</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>264.8</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>440.6</v>
+        <v>0</v>
       </c>
       <c r="H11">
-        <v>1370.3</v>
+        <v>0</v>
       </c>
       <c r="I11">
-        <v>1738.5</v>
+        <v>0</v>
       </c>
       <c r="J11">
-        <v>8.66</v>
+        <v>0</v>
       </c>
       <c r="K11">
-        <v>4.55</v>
+        <v>0</v>
       </c>
       <c r="L11">
-        <v>4.76</v>
+        <v>0</v>
       </c>
       <c r="M11">
-        <v>5.86</v>
+        <v>0</v>
       </c>
       <c r="N11">
-        <v>3.8370000000000002</v>
+        <v>0</v>
       </c>
       <c r="O11">
-        <v>353.9</v>
+        <v>0</v>
       </c>
       <c r="P11">
-        <v>201.8</v>
+        <v>0</v>
       </c>
       <c r="Q11">
-        <v>135.5</v>
+        <v>0</v>
       </c>
       <c r="R11">
-        <v>8.26</v>
+        <v>0</v>
       </c>
       <c r="S11">
-        <v>19.62</v>
+        <v>0</v>
       </c>
       <c r="T11">
-        <v>63.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -4439,61 +4439,61 @@
         <v>2009</v>
       </c>
       <c r="B12">
-        <v>347.2</v>
+        <v>0</v>
       </c>
       <c r="C12">
-        <v>1785.1</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>1.0229999999999999</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>104.7</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>301.10000000000002</v>
+        <v>0</v>
       </c>
       <c r="G12">
-        <v>569.5</v>
+        <v>0</v>
       </c>
       <c r="H12">
-        <v>1608</v>
+        <v>0</v>
       </c>
       <c r="I12">
-        <v>1839.1</v>
+        <v>0</v>
       </c>
       <c r="J12">
-        <v>10.14</v>
+        <v>0</v>
       </c>
       <c r="K12">
-        <v>6.98</v>
+        <v>0</v>
       </c>
       <c r="L12">
-        <v>7.53</v>
+        <v>0</v>
       </c>
       <c r="M12">
-        <v>5.97</v>
+        <v>0</v>
       </c>
       <c r="N12">
-        <v>4.1529999999999996</v>
+        <v>0</v>
       </c>
       <c r="O12">
-        <v>354.7</v>
+        <v>0</v>
       </c>
       <c r="P12">
-        <v>230</v>
+        <v>0</v>
       </c>
       <c r="Q12">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="R12">
-        <v>12.52</v>
+        <v>0</v>
       </c>
       <c r="S12">
-        <v>23.31</v>
+        <v>0</v>
       </c>
       <c r="T12">
-        <v>75.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -4501,61 +4501,61 @@
         <v>2010</v>
       </c>
       <c r="B13">
-        <v>364.1</v>
+        <v>0</v>
       </c>
       <c r="C13">
-        <v>2112.6</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>0.98199999999999998</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>144.19999999999999</v>
+        <v>0</v>
       </c>
       <c r="F13">
-        <v>330.6</v>
+        <v>0</v>
       </c>
       <c r="G13">
-        <v>649.20000000000005</v>
+        <v>0</v>
       </c>
       <c r="H13">
-        <v>1701.1</v>
+        <v>0</v>
       </c>
       <c r="I13">
-        <v>1920.7</v>
+        <v>0</v>
       </c>
       <c r="J13">
-        <v>10.95</v>
+        <v>0</v>
       </c>
       <c r="K13">
-        <v>8.64</v>
+        <v>0</v>
       </c>
       <c r="L13">
-        <v>10.15</v>
+        <v>0</v>
       </c>
       <c r="M13">
-        <v>8.1</v>
+        <v>0</v>
       </c>
       <c r="N13">
-        <v>4.452</v>
+        <v>0</v>
       </c>
       <c r="O13">
-        <v>378.7</v>
+        <v>0</v>
       </c>
       <c r="P13">
-        <v>244.7</v>
+        <v>0</v>
       </c>
       <c r="Q13">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="R13">
-        <v>13.92</v>
+        <v>0</v>
       </c>
       <c r="S13">
-        <v>27.91</v>
+        <v>0</v>
       </c>
       <c r="T13">
-        <v>88.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
@@ -4563,61 +4563,61 @@
         <v>2011</v>
       </c>
       <c r="B14">
-        <v>389.1</v>
+        <v>0</v>
       </c>
       <c r="C14">
-        <v>2149.5</v>
+        <v>0</v>
       </c>
       <c r="D14">
-        <v>1.0269999999999999</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>189.7</v>
+        <v>0</v>
       </c>
       <c r="F14">
-        <v>356.2</v>
+        <v>0</v>
       </c>
       <c r="G14">
-        <v>743</v>
+        <v>0</v>
       </c>
       <c r="H14">
-        <v>1808</v>
+        <v>0</v>
       </c>
       <c r="I14">
-        <v>1973.5</v>
+        <v>0</v>
       </c>
       <c r="J14">
-        <v>13.06</v>
+        <v>0</v>
       </c>
       <c r="K14">
-        <v>8.91</v>
+        <v>0</v>
       </c>
       <c r="L14">
-        <v>11.63</v>
+        <v>0</v>
       </c>
       <c r="M14">
-        <v>8.1999999999999993</v>
+        <v>0</v>
       </c>
       <c r="N14">
-        <v>4.7969999999999997</v>
+        <v>0</v>
       </c>
       <c r="O14">
-        <v>401.2</v>
+        <v>0</v>
       </c>
       <c r="P14">
-        <v>255.7</v>
+        <v>0</v>
       </c>
       <c r="Q14">
-        <v>201.5</v>
+        <v>0</v>
       </c>
       <c r="R14">
-        <v>17.22</v>
+        <v>0</v>
       </c>
       <c r="S14">
-        <v>30.95</v>
+        <v>0</v>
       </c>
       <c r="T14">
-        <v>95.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
@@ -4625,61 +4625,61 @@
         <v>2012</v>
       </c>
       <c r="B15">
-        <v>404.8</v>
+        <v>0</v>
       </c>
       <c r="C15">
-        <v>2227.4</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>1.7629999999999999</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>210</v>
+        <v>0</v>
       </c>
       <c r="F15">
-        <v>305.10000000000002</v>
+        <v>0</v>
       </c>
       <c r="G15">
-        <v>889.9</v>
+        <v>0</v>
       </c>
       <c r="H15">
-        <v>1892.5</v>
+        <v>0</v>
       </c>
       <c r="I15">
-        <v>2054.8000000000002</v>
+        <v>0</v>
       </c>
       <c r="J15">
-        <v>15.62</v>
+        <v>0</v>
       </c>
       <c r="K15">
-        <v>9.3000000000000007</v>
+        <v>0</v>
       </c>
       <c r="L15">
-        <v>13.26</v>
+        <v>0</v>
       </c>
       <c r="M15">
-        <v>9.6999999999999993</v>
+        <v>0</v>
       </c>
       <c r="N15">
-        <v>4.8550000000000004</v>
+        <v>0</v>
       </c>
       <c r="O15">
-        <v>432.4</v>
+        <v>0</v>
       </c>
       <c r="P15">
-        <v>261</v>
+        <v>0</v>
       </c>
       <c r="Q15">
-        <v>217.2</v>
+        <v>0</v>
       </c>
       <c r="R15">
-        <v>19.420000000000002</v>
+        <v>0</v>
       </c>
       <c r="S15">
-        <v>38.03</v>
+        <v>0</v>
       </c>
       <c r="T15">
-        <v>107.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -4687,61 +4687,61 @@
         <v>2013</v>
       </c>
       <c r="B16">
-        <v>414.4</v>
+        <v>0</v>
       </c>
       <c r="C16">
-        <v>2213</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>1.9339999999999999</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>215.4</v>
+        <v>0</v>
       </c>
       <c r="F16">
-        <v>320.5</v>
+        <v>0</v>
       </c>
       <c r="G16">
-        <v>977.3</v>
+        <v>0</v>
       </c>
       <c r="H16">
-        <v>1977.7</v>
+        <v>0</v>
       </c>
       <c r="I16">
-        <v>2136.1999999999998</v>
+        <v>0</v>
       </c>
       <c r="J16">
-        <v>18.71</v>
+        <v>0</v>
       </c>
       <c r="K16">
-        <v>9.18</v>
+        <v>0</v>
       </c>
       <c r="L16">
-        <v>13.55</v>
+        <v>0</v>
       </c>
       <c r="M16">
-        <v>11.01</v>
+        <v>0</v>
       </c>
       <c r="N16">
-        <v>5.2270000000000003</v>
+        <v>0</v>
       </c>
       <c r="O16">
-        <v>446.8</v>
+        <v>0</v>
       </c>
       <c r="P16">
-        <v>263.2</v>
+        <v>0</v>
       </c>
       <c r="Q16">
-        <v>224.1</v>
+        <v>0</v>
       </c>
       <c r="R16">
-        <v>25.52</v>
+        <v>0</v>
       </c>
       <c r="S16">
-        <v>40.68</v>
+        <v>0</v>
       </c>
       <c r="T16">
-        <v>114.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
@@ -4749,371 +4749,371 @@
         <v>2014</v>
       </c>
       <c r="B17">
-        <v>431.2</v>
+        <v>0</v>
       </c>
       <c r="C17">
-        <v>2215.1999999999998</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>2.13</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>203.4</v>
+        <v>0</v>
       </c>
       <c r="F17">
-        <v>319.60000000000002</v>
+        <v>0</v>
       </c>
       <c r="G17">
-        <v>1039.4000000000001</v>
+        <v>0</v>
       </c>
       <c r="H17">
-        <v>2039.9</v>
+        <v>0</v>
       </c>
       <c r="I17">
-        <v>2203</v>
+        <v>0</v>
       </c>
       <c r="J17">
-        <v>19.010000000000002</v>
+        <v>0</v>
       </c>
       <c r="K17">
-        <v>9.83</v>
+        <v>0</v>
       </c>
       <c r="L17">
-        <v>14.83</v>
+        <v>0</v>
       </c>
       <c r="M17">
-        <v>11.33</v>
+        <v>0</v>
       </c>
       <c r="N17">
-        <v>5.39</v>
+        <v>0</v>
       </c>
       <c r="O17">
-        <v>455.6</v>
+        <v>0</v>
       </c>
       <c r="P17">
-        <v>280</v>
+        <v>0</v>
       </c>
       <c r="Q17">
-        <v>230.1</v>
+        <v>0</v>
       </c>
       <c r="R17">
-        <v>30.22</v>
+        <v>0</v>
       </c>
       <c r="S17">
-        <v>40.799999999999997</v>
+        <v>0</v>
       </c>
       <c r="T17">
-        <v>123.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2015</v>
       </c>
-      <c r="B18">
-        <v>438.2</v>
-      </c>
-      <c r="C18">
-        <v>2185.1</v>
-      </c>
-      <c r="D18">
-        <v>2.077</v>
-      </c>
-      <c r="E18">
-        <v>201.6</v>
-      </c>
-      <c r="F18">
-        <v>311.7</v>
-      </c>
-      <c r="G18">
-        <v>1070.0999999999999</v>
-      </c>
-      <c r="H18">
-        <v>2101.3000000000002</v>
-      </c>
-      <c r="I18">
-        <v>2239.4</v>
-      </c>
-      <c r="J18">
-        <v>19.16</v>
-      </c>
-      <c r="K18">
-        <v>9.11</v>
-      </c>
-      <c r="L18">
-        <v>15.88</v>
-      </c>
-      <c r="M18">
-        <v>11.45</v>
-      </c>
-      <c r="N18">
-        <v>5.5860000000000003</v>
-      </c>
-      <c r="O18">
-        <v>446</v>
-      </c>
-      <c r="P18">
-        <v>292.3</v>
-      </c>
-      <c r="Q18">
-        <v>235.7</v>
-      </c>
-      <c r="R18">
-        <v>32.090000000000003</v>
-      </c>
-      <c r="S18">
-        <v>41.38</v>
-      </c>
-      <c r="T18">
-        <v>134.5</v>
+      <c r="B18" s="2">
+        <v>12641</v>
+      </c>
+      <c r="C18" s="2">
+        <v>115625</v>
+      </c>
+      <c r="D18" s="2">
+        <v>48</v>
+      </c>
+      <c r="E18" s="2">
+        <v>7583</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <v>56817</v>
+      </c>
+      <c r="H18" s="2">
+        <v>91767</v>
+      </c>
+      <c r="I18" s="2">
+        <v>79209</v>
+      </c>
+      <c r="J18" s="2">
+        <v>285</v>
+      </c>
+      <c r="K18" s="2">
+        <v>684</v>
+      </c>
+      <c r="L18" s="2">
+        <v>1107</v>
+      </c>
+      <c r="M18" s="2">
+        <v>1115</v>
+      </c>
+      <c r="N18" s="2">
+        <v>282</v>
+      </c>
+      <c r="O18" s="2">
+        <v>25612</v>
+      </c>
+      <c r="P18" s="2">
+        <v>12641</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>11220</v>
+      </c>
+      <c r="R18" s="2">
+        <v>2228</v>
+      </c>
+      <c r="S18" s="2">
+        <v>4622</v>
+      </c>
+      <c r="T18" s="2">
+        <v>8086</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2016</v>
       </c>
-      <c r="B19">
-        <v>451.3</v>
-      </c>
-      <c r="C19">
-        <v>2169</v>
-      </c>
-      <c r="D19">
-        <v>2.2160000000000002</v>
-      </c>
-      <c r="E19">
-        <v>200.6</v>
-      </c>
-      <c r="F19">
-        <v>315</v>
-      </c>
-      <c r="G19">
-        <v>1104.5999999999999</v>
-      </c>
-      <c r="H19">
-        <v>2188.5</v>
-      </c>
-      <c r="I19">
-        <v>2285.6</v>
-      </c>
-      <c r="J19">
-        <v>19.510000000000002</v>
-      </c>
-      <c r="K19">
-        <v>10.25</v>
-      </c>
-      <c r="L19">
-        <v>15.45</v>
-      </c>
-      <c r="M19">
-        <v>11.02</v>
-      </c>
-      <c r="N19">
-        <v>5.74</v>
-      </c>
-      <c r="O19">
-        <v>438.4</v>
-      </c>
-      <c r="P19">
-        <v>296.3</v>
-      </c>
-      <c r="Q19">
-        <v>245.2</v>
-      </c>
-      <c r="R19">
-        <v>31.76</v>
-      </c>
-      <c r="S19">
-        <v>42.16</v>
-      </c>
-      <c r="T19">
-        <v>137.4</v>
+      <c r="B19" s="2">
+        <v>20559</v>
+      </c>
+      <c r="C19" s="2">
+        <v>188321</v>
+      </c>
+      <c r="D19" s="2">
+        <v>18</v>
+      </c>
+      <c r="E19" s="2">
+        <v>10982</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0</v>
+      </c>
+      <c r="G19" s="2">
+        <v>93514</v>
+      </c>
+      <c r="H19" s="2">
+        <v>149100</v>
+      </c>
+      <c r="I19" s="2">
+        <v>130398</v>
+      </c>
+      <c r="J19" s="2">
+        <v>-37</v>
+      </c>
+      <c r="K19" s="2">
+        <v>628</v>
+      </c>
+      <c r="L19" s="2">
+        <v>1157</v>
+      </c>
+      <c r="M19" s="2">
+        <v>628</v>
+      </c>
+      <c r="N19" s="2">
+        <v>525</v>
+      </c>
+      <c r="O19" s="2">
+        <v>42212</v>
+      </c>
+      <c r="P19" s="2">
+        <v>20559</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>13390</v>
+      </c>
+      <c r="R19" s="2">
+        <v>2705</v>
+      </c>
+      <c r="S19" s="2">
+        <v>3534</v>
+      </c>
+      <c r="T19" s="2">
+        <v>13205</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2017</v>
       </c>
-      <c r="B20">
-        <v>453.8</v>
-      </c>
-      <c r="C20">
-        <v>2118.6999999999998</v>
-      </c>
-      <c r="D20">
-        <v>2.2189999999999999</v>
-      </c>
-      <c r="E20">
-        <v>201.3</v>
-      </c>
-      <c r="F20">
-        <v>317.5</v>
-      </c>
-      <c r="G20">
-        <v>1145.0999999999999</v>
-      </c>
-      <c r="H20">
-        <v>2258.6</v>
-      </c>
-      <c r="I20">
-        <v>2329.6</v>
-      </c>
-      <c r="J20">
-        <v>18.809999999999999</v>
-      </c>
-      <c r="K20">
-        <v>10.52</v>
-      </c>
-      <c r="L20">
-        <v>16.54</v>
-      </c>
-      <c r="M20">
-        <v>12.7</v>
-      </c>
-      <c r="N20">
-        <v>5.6779999999999999</v>
-      </c>
-      <c r="O20">
-        <v>420.1</v>
-      </c>
-      <c r="P20">
-        <v>289.89999999999998</v>
-      </c>
-      <c r="Q20">
-        <v>247.2</v>
-      </c>
-      <c r="R20">
-        <v>31.86</v>
-      </c>
-      <c r="S20">
-        <v>43.37</v>
-      </c>
-      <c r="T20">
-        <v>138.4</v>
+      <c r="B20" s="2">
+        <v>18761</v>
+      </c>
+      <c r="C20" s="2">
+        <v>155372</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2">
+        <v>6719</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0</v>
+      </c>
+      <c r="G20" s="2">
+        <v>79919</v>
+      </c>
+      <c r="H20" s="2">
+        <v>134836</v>
+      </c>
+      <c r="I20" s="2">
+        <v>117120</v>
+      </c>
+      <c r="J20" s="2">
+        <v>-35</v>
+      </c>
+      <c r="K20" s="2">
+        <v>430</v>
+      </c>
+      <c r="L20" s="2">
+        <v>640</v>
+      </c>
+      <c r="M20" s="2">
+        <v>642</v>
+      </c>
+      <c r="N20" s="2">
+        <v>220</v>
+      </c>
+      <c r="O20" s="2">
+        <v>34959</v>
+      </c>
+      <c r="P20" s="2">
+        <v>18761</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>6464</v>
+      </c>
+      <c r="R20" s="2">
+        <v>1974</v>
+      </c>
+      <c r="S20" s="2">
+        <v>2627</v>
+      </c>
+      <c r="T20" s="2">
+        <v>7872</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2018</v>
       </c>
-      <c r="B21">
-        <v>459.1</v>
-      </c>
-      <c r="C21">
-        <v>2068.6</v>
-      </c>
-      <c r="D21">
-        <v>2.1739999999999999</v>
-      </c>
-      <c r="E21">
-        <v>205.9</v>
-      </c>
-      <c r="F21">
-        <v>334.7</v>
-      </c>
-      <c r="G21">
-        <v>1173.3</v>
-      </c>
-      <c r="H21">
-        <v>2314.9</v>
-      </c>
-      <c r="I21">
-        <v>2380.9</v>
-      </c>
-      <c r="J21">
-        <v>21.26</v>
-      </c>
-      <c r="K21">
-        <v>10.82</v>
-      </c>
-      <c r="L21">
-        <v>15.32</v>
-      </c>
-      <c r="M21">
-        <v>12.61</v>
-      </c>
-      <c r="N21">
-        <v>5.6440000000000001</v>
-      </c>
-      <c r="O21">
-        <v>405.5</v>
-      </c>
-      <c r="P21">
-        <v>285.3</v>
-      </c>
-      <c r="Q21">
-        <v>249.3</v>
-      </c>
-      <c r="R21">
-        <v>32.22</v>
-      </c>
-      <c r="S21">
-        <v>44.32</v>
-      </c>
-      <c r="T21">
-        <v>139.30000000000001</v>
+      <c r="B21" s="2">
+        <v>6228</v>
+      </c>
+      <c r="C21" s="2">
+        <v>59239</v>
+      </c>
+      <c r="D21" s="2">
+        <v>-58</v>
+      </c>
+      <c r="E21" s="2">
+        <v>4851</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0</v>
+      </c>
+      <c r="G21" s="2">
+        <v>30571</v>
+      </c>
+      <c r="H21" s="2">
+        <v>44554</v>
+      </c>
+      <c r="I21" s="2">
+        <v>38627</v>
+      </c>
+      <c r="J21" s="2">
+        <v>464</v>
+      </c>
+      <c r="K21" s="2">
+        <v>333</v>
+      </c>
+      <c r="L21" s="2">
+        <v>260</v>
+      </c>
+      <c r="M21" s="2">
+        <v>228</v>
+      </c>
+      <c r="N21" s="2">
+        <v>127</v>
+      </c>
+      <c r="O21" s="2">
+        <v>12400</v>
+      </c>
+      <c r="P21" s="2">
+        <v>6228</v>
+      </c>
+      <c r="Q21" s="2">
+        <v>5772</v>
+      </c>
+      <c r="R21" s="2">
+        <v>1039</v>
+      </c>
+      <c r="S21" s="2">
+        <v>902</v>
+      </c>
+      <c r="T21" s="2">
+        <v>3970</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2019</v>
       </c>
-      <c r="B22">
-        <v>467.2</v>
-      </c>
-      <c r="C22">
-        <v>2053</v>
-      </c>
-      <c r="D22">
-        <v>2.36</v>
-      </c>
-      <c r="E22">
-        <v>204</v>
-      </c>
-      <c r="F22">
-        <v>331.1</v>
-      </c>
-      <c r="G22">
-        <v>1188.9000000000001</v>
-      </c>
-      <c r="H22">
-        <v>2380.1</v>
-      </c>
-      <c r="I22">
-        <v>2409.8000000000002</v>
-      </c>
-      <c r="J22">
-        <v>20.96</v>
-      </c>
-      <c r="K22">
-        <v>11.24</v>
-      </c>
-      <c r="L22">
-        <v>17.52</v>
-      </c>
-      <c r="M22">
-        <v>14.01</v>
-      </c>
-      <c r="N22">
-        <v>5.6959999999999997</v>
-      </c>
-      <c r="O22">
-        <v>394.6</v>
-      </c>
-      <c r="P22">
-        <v>280.39999999999998</v>
-      </c>
-      <c r="Q22">
-        <v>250</v>
-      </c>
-      <c r="R22">
-        <v>31.74</v>
-      </c>
-      <c r="S22">
-        <v>45.2</v>
-      </c>
-      <c r="T22">
-        <v>142.5</v>
+      <c r="B22" s="2">
+        <v>1387</v>
+      </c>
+      <c r="C22" s="2">
+        <v>9276</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2">
+        <v>2591</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0</v>
+      </c>
+      <c r="G22" s="2">
+        <v>-1819</v>
+      </c>
+      <c r="H22" s="2">
+        <v>4904</v>
+      </c>
+      <c r="I22" s="2">
+        <v>-1566</v>
+      </c>
+      <c r="J22" s="2">
+        <v>1267</v>
+      </c>
+      <c r="K22" s="2">
+        <v>282</v>
+      </c>
+      <c r="L22" s="2">
+        <v>541</v>
+      </c>
+      <c r="M22" s="2">
+        <v>107</v>
+      </c>
+      <c r="N22" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O22" s="2">
+        <v>-421</v>
+      </c>
+      <c r="P22" s="2">
+        <v>1387</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>4343</v>
+      </c>
+      <c r="R22" s="2">
+        <v>263</v>
+      </c>
+      <c r="S22" s="2">
+        <v>837</v>
+      </c>
+      <c r="T22" s="2">
+        <v>751</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some changes in the code, PSPP as percentage of GDP added
</commit_message>
<xml_diff>
--- a/input/full_data.xlsx
+++ b/input/full_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Viktor\Dropbox\GitHub\macroX_sovereign-yield-spreads\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C901E41C-5025-40E3-A903-5CB359BF99D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9173D5EA-F89D-4FB7-8F4E-D3407C5AEBBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="10" xr2:uid="{6BD05D62-9C8D-4B00-B784-FD56BE4060DE}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="13" xr2:uid="{6BD05D62-9C8D-4B00-B784-FD56BE4060DE}"/>
   </bookViews>
   <sheets>
     <sheet name="bb" sheetId="3" r:id="rId1"/>
@@ -3746,8 +3746,8 @@
   </sheetPr>
   <dimension ref="A1:T22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7892,8 +7892,8 @@
   </sheetPr>
   <dimension ref="A1:T22"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
correction us value 1999
</commit_message>
<xml_diff>
--- a/input/full_data.xlsx
+++ b/input/full_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Viktor\Dropbox\GitHub\macroX_sovereign-yield-spreads\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1018DFDB-7382-4BA7-978D-665BF9660E1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BEB7EBE-2872-45FA-AD3E-6FE139D0EE7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" firstSheet="10" activeTab="24" xr2:uid="{6BD05D62-9C8D-4B00-B784-FD56BE4060DE}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" firstSheet="10" activeTab="19" xr2:uid="{6BD05D62-9C8D-4B00-B784-FD56BE4060DE}"/>
   </bookViews>
   <sheets>
     <sheet name="bb" sheetId="3" r:id="rId1"/>
@@ -18327,8 +18327,8 @@
   </sheetPr>
   <dimension ref="A1:T23"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N43" sqref="N43"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18462,61 +18462,61 @@
         <v>1999</v>
       </c>
       <c r="B3">
-        <v>1275.8600000000008</v>
+        <v>5.0831075697211183</v>
       </c>
       <c r="C3">
-        <v>1275.8600000000008</v>
+        <v>5.0831075697211183</v>
       </c>
       <c r="D3">
-        <v>1275.8599999999999</v>
+        <v>5.0831075697211201</v>
       </c>
       <c r="E3">
-        <v>1275.8599999999999</v>
+        <v>5.0831075697211201</v>
       </c>
       <c r="F3">
-        <v>1275.8599999999999</v>
+        <v>5.0831075697211201</v>
       </c>
       <c r="G3">
-        <v>1275.8599999999999</v>
+        <v>5.0831075697211201</v>
       </c>
       <c r="H3">
-        <v>1275.8599999999999</v>
+        <v>5.0831075697211201</v>
       </c>
       <c r="I3">
-        <v>1275.8599999999999</v>
+        <v>5.0831075697211201</v>
       </c>
       <c r="J3">
-        <v>1275.8599999999999</v>
+        <v>5.0831075697211201</v>
       </c>
       <c r="K3">
-        <v>1275.8599999999999</v>
+        <v>5.0831075697211201</v>
       </c>
       <c r="L3">
-        <v>1275.8599999999999</v>
+        <v>5.0831075697211201</v>
       </c>
       <c r="M3">
-        <v>1275.8599999999999</v>
+        <v>5.0831075697211201</v>
       </c>
       <c r="N3">
-        <v>1275.8599999999999</v>
+        <v>5.0831075697211201</v>
       </c>
       <c r="O3">
-        <v>1275.8599999999999</v>
+        <v>5.0831075697211201</v>
       </c>
       <c r="P3">
-        <v>1275.8599999999999</v>
+        <v>5.0831075697211201</v>
       </c>
       <c r="Q3">
-        <v>1275.8599999999999</v>
+        <v>5.0831075697211201</v>
       </c>
       <c r="R3">
-        <v>1275.8599999999999</v>
+        <v>5.0831075697211201</v>
       </c>
       <c r="S3">
-        <v>1275.8599999999999</v>
+        <v>5.0831075697211201</v>
       </c>
       <c r="T3">
-        <v>1275.8599999999999</v>
+        <v>5.0831075697211201</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -25547,7 +25547,7 @@
   </sheetPr>
   <dimension ref="A1:T23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="R32" sqref="R32"/>
     </sheetView>
   </sheetViews>

</xml_diff>